<commit_message>
Updated some files and added Programming Basics on C# and JavaScript
</commit_message>
<xml_diff>
--- a/Professional Modules/Web Basics/Web Fundamentals - HTML5/Web-Basics-Module-Schedule-Jan-2017.xlsx
+++ b/Professional Modules/Web Basics/Web Fundamentals - HTML5/Web-Basics-Module-Schedule-Jan-2017.xlsx
@@ -1164,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="85.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,7 +1269,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="A5" s="23">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Added HTML Strucure - Exercises
</commit_message>
<xml_diff>
--- a/Professional Modules/Web Basics/Web Fundamentals - HTML5/Web-Basics-Module-Schedule-Jan-2017.xlsx
+++ b/Professional Modules/Web Basics/Web Fundamentals - HTML5/Web-Basics-Module-Schedule-Jan-2017.xlsx
@@ -1165,7 +1165,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="85.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1319,7 +1319,7 @@
         <f>IF(OR(Table132[[#This Row],[Day]]="Tuesday", Table132[[#This Row],[Day]]="Thursday"), "14:00-18:00", "18:00-22:00")</f>
         <v>18:00-22:00</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="26">
         <f>Table132[[#This Row],[Date]]+5</f>
         <v>42774</v>
       </c>

</xml_diff>

<commit_message>
Added some files in Professional Module
</commit_message>
<xml_diff>
--- a/Professional Modules/Web Basics/Web Fundamentals - HTML5/Web-Basics-Module-Schedule-Jan-2017.xlsx
+++ b/Professional Modules/Web Basics/Web Fundamentals - HTML5/Web-Basics-Module-Schedule-Jan-2017.xlsx
@@ -483,7 +483,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -504,6 +504,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -532,7 +538,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -618,6 +624,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1165,7 +1186,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="85.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,25 +1318,25 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+      <c r="A6" s="23">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="C6" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="26">
         <f>D5+2</f>
         <v>42769</v>
       </c>
-      <c r="E6" s="8" t="str">
+      <c r="E6" s="27" t="str">
         <f>TEXT(Table132[[#This Row],[Date]],"dddd")</f>
         <v>Friday</v>
       </c>
-      <c r="F6" s="8" t="str">
+      <c r="F6" s="27" t="str">
         <f>IF(OR(Table132[[#This Row],[Day]]="Tuesday", Table132[[#This Row],[Day]]="Thursday"), "14:00-18:00", "18:00-22:00")</f>
         <v>18:00-22:00</v>
       </c>
@@ -1325,29 +1346,29 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9">
+      <c r="A7" s="30">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="C7" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="33">
         <f t="shared" ref="D7" si="1">D5+7</f>
         <v>42774</v>
       </c>
-      <c r="E7" s="8" t="str">
+      <c r="E7" s="34" t="str">
         <f>TEXT(Table132[[#This Row],[Date]],"dddd")</f>
         <v>Wednesday</v>
       </c>
-      <c r="F7" s="8" t="str">
+      <c r="F7" s="34" t="str">
         <f>IF(OR(Table132[[#This Row],[Day]]="Tuesday", Table132[[#This Row],[Day]]="Thursday"), "14:00-18:00", "18:00-22:00")</f>
         <v>18:00-22:00</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="33">
         <f>Table132[[#This Row],[Date]]+5</f>
         <v>42779</v>
       </c>

</xml_diff>